<commit_message>
parallel: <<lab3>>: update table
</commit_message>
<xml_diff>
--- a/Parallel and distributed systems/parallel/lab3/lab3_results.xlsx
+++ b/Parallel and distributed systems/parallel/lab3/lab3_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t xml:space="preserve">Тип задачи</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.025944</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.035772</t>
@@ -90,7 +87,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,61 +110,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Mangal"/>
-      <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
@@ -197,77 +139,20 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -278,7 +163,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,37 +187,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,27 +209,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,11 +241,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +253,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,95 +261,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Заголовок" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -492,7 +285,7 @@
   <dimension ref="B2:Q21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -699,18 +492,13 @@
         <f aca="false">E6/F7</f>
         <v>1.12628608639028</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="H7" s="9" t="n">
+        <f aca="false">G7/2</f>
+        <v>0.56314304319514</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -766,7 +554,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="8" t="n">
         <v>0.020154</v>
@@ -846,7 +634,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="8" t="n">
         <v>0.112497</v>
@@ -926,7 +714,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="14"/>
       <c r="E13" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="8" t="n">
         <v>0.066312</v>
@@ -1006,7 +794,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="8" t="n">
         <v>0.051445</v>
@@ -1086,7 +874,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="8" t="n">
         <v>0.200659</v>

</xml_diff>